<commit_message>
Imagens de formação de voo substituidas
</commit_message>
<xml_diff>
--- a/Teste TCC.xlsx
+++ b/Teste TCC.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="51">
   <si>
     <t>Tx Error</t>
   </si>
@@ -200,6 +200,39 @@
   <si>
     <t>Throughput</t>
   </si>
+  <si>
+    <t>Teste Ar - 500m</t>
+  </si>
+  <si>
+    <t>Teste Ar - 600m</t>
+  </si>
+  <si>
+    <t>Teste Ar - 700m</t>
+  </si>
+  <si>
+    <t>Teste Ar - 800m</t>
+  </si>
+  <si>
+    <t>Teste Ar - 900m</t>
+  </si>
+  <si>
+    <t>Teste Ar - 1000m</t>
+  </si>
+  <si>
+    <t>Teste Ar - 1100m</t>
+  </si>
+  <si>
+    <t>400m</t>
+  </si>
+  <si>
+    <t>500m</t>
+  </si>
+  <si>
+    <t>600m</t>
+  </si>
+  <si>
+    <t>700m</t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -312,26 +345,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -355,6 +368,17 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -405,6 +429,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,21 +442,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -578,9 +602,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$C$17:$C$23</c:f>
+              <c:f>Sheet2!$C$17:$C$27</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>50m</c:v>
                 </c:pt>
@@ -602,15 +626,27 @@
                 <c:pt idx="6">
                   <c:v>350m</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>400m</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500m</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600m</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700m</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$F$17:$F$23</c:f>
+              <c:f>Sheet2!$F$17:$F$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-40.0</c:v>
                 </c:pt>
@@ -632,6 +668,18 @@
                 <c:pt idx="6">
                   <c:v>-50.2</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>-56.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-53.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-46.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-46.4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -641,7 +689,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Remote</c:v>
+            <c:v>remote</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
@@ -657,9 +705,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$C$17:$C$23</c:f>
+              <c:f>Sheet2!$C$17:$C$27</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>50m</c:v>
                 </c:pt>
@@ -681,15 +729,27 @@
                 <c:pt idx="6">
                   <c:v>350m</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>400m</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500m</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600m</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700m</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$17:$G$23</c:f>
+              <c:f>Sheet2!$G$17:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>-40.8</c:v>
                 </c:pt>
@@ -710,6 +770,18 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-51.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-58.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-56.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-48.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-48.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -740,11 +812,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="2070956160"/>
-        <c:axId val="2136149472"/>
+        <c:axId val="-2108472336"/>
+        <c:axId val="-2108469104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2070956160"/>
+        <c:axId val="-2108472336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -787,7 +859,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2136149472"/>
+        <c:crossAx val="-2108469104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -795,7 +867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2136149472"/>
+        <c:axId val="-2108469104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,7 +904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2070956160"/>
+        <c:crossAx val="-2108472336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1028,7 +1100,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>taxa de transferência</c:v>
+            <c:v>Taxa de Transferência</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
@@ -1044,9 +1116,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$C$17:$C$23</c:f>
+              <c:f>Sheet2!$C$17:$C$27</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>50m</c:v>
                 </c:pt>
@@ -1068,15 +1140,27 @@
                 <c:pt idx="6">
                   <c:v>350m</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>400m</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500m</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600m</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700m</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$I$17:$I$23</c:f>
+              <c:f>Sheet2!$I$17:$I$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>10.226</c:v>
                 </c:pt>
@@ -1097,6 +1181,18 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9.966</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.916</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.852</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.276</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32.494</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,11 +1223,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-2079788640"/>
-        <c:axId val="-2124865024"/>
+        <c:axId val="-2139883424"/>
+        <c:axId val="-2139880176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2079788640"/>
+        <c:axId val="-2139883424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124865024"/>
+        <c:crossAx val="-2139880176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1182,7 +1278,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124865024"/>
+        <c:axId val="-2139880176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079788640"/>
+        <c:crossAx val="-2139883424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1525,11 +1621,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-2072199984"/>
-        <c:axId val="-2074314944"/>
+        <c:axId val="-2139815792"/>
+        <c:axId val="-2139812560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2072199984"/>
+        <c:axId val="-2139815792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074314944"/>
+        <c:crossAx val="-2139812560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1580,7 +1676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074314944"/>
+        <c:axId val="-2139812560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072199984"/>
+        <c:crossAx val="-2139815792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1874,11 +1970,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="-2123601760"/>
-        <c:axId val="-2074855424"/>
+        <c:axId val="-2139779680"/>
+        <c:axId val="-2139776448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2123601760"/>
+        <c:axId val="-2139779680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1921,7 +2017,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2074855424"/>
+        <c:crossAx val="-2139776448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1929,7 +2025,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2074855424"/>
+        <c:axId val="-2139776448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1966,7 +2062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123601760"/>
+        <c:crossAx val="-2139779680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4767,8 +4863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:CW35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
-      <selection activeCell="W41" sqref="W41"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4783,387 +4879,511 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="W2" s="8" t="s">
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="W2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AG2" s="8" t="s">
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AG2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AQ2" s="8" t="s">
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AQ2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
-      <c r="CO2" s="8" t="s">
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
+      <c r="AW2" s="9"/>
+      <c r="AX2" s="9"/>
+      <c r="AY2" s="9"/>
+      <c r="BA2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB2" s="9"/>
+      <c r="BC2" s="9"/>
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+      <c r="BH2" s="9"/>
+      <c r="BI2" s="9"/>
+      <c r="BK2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL2" s="9"/>
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="9"/>
+      <c r="BO2" s="9"/>
+      <c r="BP2" s="9"/>
+      <c r="BQ2" s="9"/>
+      <c r="BR2" s="9"/>
+      <c r="BS2" s="9"/>
+      <c r="CO2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="CP2" s="8"/>
-      <c r="CQ2" s="8"/>
-      <c r="CR2" s="8"/>
-      <c r="CS2" s="8"/>
-      <c r="CT2" s="8"/>
-      <c r="CU2" s="8"/>
-      <c r="CV2" s="8"/>
-      <c r="CW2" s="8"/>
+      <c r="CP2" s="9"/>
+      <c r="CQ2" s="9"/>
+      <c r="CR2" s="9"/>
+      <c r="CS2" s="9"/>
+      <c r="CT2" s="9"/>
+      <c r="CU2" s="9"/>
+      <c r="CV2" s="9"/>
+      <c r="CW2" s="9"/>
     </row>
     <row r="3" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="M3" s="7" t="s">
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="M3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="8" t="s">
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="W3" s="7" t="s">
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="W3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="8" t="s">
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AG3" s="7" t="s">
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AG3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="8" t="s">
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AN3" s="8"/>
-      <c r="AO3" s="8"/>
-      <c r="AQ3" s="7" t="s">
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9"/>
+      <c r="AQ3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AR3" s="7"/>
-      <c r="AS3" s="7"/>
-      <c r="AT3" s="7"/>
-      <c r="AU3" s="7"/>
-      <c r="AV3" s="7"/>
-      <c r="AW3" s="8" t="s">
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AX3" s="8"/>
-      <c r="AY3" s="8"/>
-      <c r="CO3" s="7" t="s">
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="9"/>
+      <c r="BA3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="CP3" s="7"/>
-      <c r="CQ3" s="7"/>
-      <c r="CR3" s="7"/>
-      <c r="CS3" s="7"/>
-      <c r="CT3" s="7"/>
-      <c r="CU3" s="8" t="s">
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CV3" s="8"/>
-      <c r="CW3" s="8"/>
+      <c r="BH3" s="9"/>
+      <c r="BI3" s="9"/>
+      <c r="BK3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR3" s="9"/>
+      <c r="BS3" s="9"/>
+      <c r="CO3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="CP3" s="8"/>
+      <c r="CQ3" s="8"/>
+      <c r="CR3" s="8"/>
+      <c r="CS3" s="8"/>
+      <c r="CT3" s="8"/>
+      <c r="CU3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="CV3" s="9"/>
+      <c r="CW3" s="9"/>
     </row>
     <row r="4" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="7" t="s">
+      <c r="N4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="7" t="s">
+      <c r="R4" s="9"/>
+      <c r="S4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="T4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="W4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="X4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="7" t="s">
+      <c r="X4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AA4" s="8" t="s">
+      <c r="AA4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="7" t="s">
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AD4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="7" t="s">
+      <c r="AE4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AG4" s="7" t="s">
+      <c r="AG4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AH4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AH4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AJ4" s="7" t="s">
+      <c r="AJ4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AK4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AL4" s="8"/>
-      <c r="AM4" s="7" t="s">
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AN4" s="7" t="s">
+      <c r="AN4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AO4" s="7" t="s">
+      <c r="AO4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AQ4" s="7" t="s">
+      <c r="AQ4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AR4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AS4" s="7" t="s">
+      <c r="AR4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AT4" s="7" t="s">
+      <c r="AT4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AU4" s="8" t="s">
+      <c r="AU4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AV4" s="8"/>
-      <c r="AW4" s="7" t="s">
+      <c r="AV4" s="9"/>
+      <c r="AW4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AX4" s="7" t="s">
+      <c r="AX4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AY4" s="7" t="s">
+      <c r="AY4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="CO4" s="7" t="s">
+      <c r="BA4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="CP4" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="CQ4" s="7" t="s">
+      <c r="BB4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="CR4" s="7" t="s">
+      <c r="BD4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="CS4" s="8" t="s">
+      <c r="BE4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="CT4" s="8"/>
-      <c r="CU4" s="7" t="s">
+      <c r="BF4" s="9"/>
+      <c r="BG4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="CV4" s="7" t="s">
+      <c r="BH4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="CW4" s="7" t="s">
+      <c r="BI4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP4" s="9"/>
+      <c r="BQ4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="CO4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="CP4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="CQ4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="CR4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="CS4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT4" s="9"/>
+      <c r="CU4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="CV4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="CW4" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
       <c r="Q5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
       <c r="AA5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
       <c r="AK5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AL5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AQ5" s="7"/>
-      <c r="AR5" s="7"/>
-      <c r="AS5" s="7"/>
-      <c r="AT5" s="7"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
       <c r="AU5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AV5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AW5" s="7"/>
-      <c r="AX5" s="7"/>
-      <c r="AY5" s="7"/>
-      <c r="CO5" s="7"/>
-      <c r="CP5" s="7"/>
-      <c r="CQ5" s="7"/>
-      <c r="CR5" s="7"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+      <c r="BA5" s="8"/>
+      <c r="BB5" s="8"/>
+      <c r="BC5" s="8"/>
+      <c r="BD5" s="8"/>
+      <c r="BE5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG5" s="8"/>
+      <c r="BH5" s="8"/>
+      <c r="BI5" s="8"/>
+      <c r="BK5" s="8"/>
+      <c r="BL5" s="8"/>
+      <c r="BM5" s="8"/>
+      <c r="BN5" s="8"/>
+      <c r="BO5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BP5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ5" s="8"/>
+      <c r="BR5" s="8"/>
+      <c r="BS5" s="8"/>
+      <c r="CO5" s="8"/>
+      <c r="CP5" s="8"/>
+      <c r="CQ5" s="8"/>
+      <c r="CR5" s="8"/>
       <c r="CS5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="CT5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CU5" s="7"/>
-      <c r="CV5" s="7"/>
-      <c r="CW5" s="7"/>
+      <c r="CU5" s="8"/>
+      <c r="CV5" s="8"/>
+      <c r="CW5" s="8"/>
     </row>
     <row r="6" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>40</v>
       </c>
       <c r="D6" s="1">
@@ -5181,7 +5401,7 @@
       <c r="H6" s="1">
         <v>-61</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="1">
@@ -5190,7 +5410,7 @@
       <c r="K6" s="1">
         <v>5.81</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="7">
         <v>40</v>
       </c>
       <c r="N6" s="1">
@@ -5208,7 +5428,7 @@
       <c r="R6" s="1">
         <v>-74</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="T6" s="1">
@@ -5217,7 +5437,7 @@
       <c r="U6" s="1">
         <v>5.2</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="7">
         <v>40</v>
       </c>
       <c r="X6" s="1">
@@ -5235,7 +5455,7 @@
       <c r="AB6" s="1">
         <v>-40</v>
       </c>
-      <c r="AC6" s="6">
+      <c r="AC6" s="7">
         <v>10</v>
       </c>
       <c r="AD6" s="1">
@@ -5244,7 +5464,7 @@
       <c r="AE6" s="1">
         <v>10.28</v>
       </c>
-      <c r="AG6" s="6">
+      <c r="AG6" s="7">
         <v>40</v>
       </c>
       <c r="AH6" s="1">
@@ -5262,7 +5482,7 @@
       <c r="AL6" s="1">
         <v>-49</v>
       </c>
-      <c r="AM6" s="6">
+      <c r="AM6" s="7">
         <v>10</v>
       </c>
       <c r="AN6" s="1">
@@ -5271,7 +5491,7 @@
       <c r="AO6" s="1">
         <v>10.4</v>
       </c>
-      <c r="AQ6" s="6">
+      <c r="AQ6" s="7">
         <v>40</v>
       </c>
       <c r="AR6" s="1">
@@ -5289,7 +5509,7 @@
       <c r="AV6" s="1">
         <v>-51</v>
       </c>
-      <c r="AW6" s="6">
+      <c r="AW6" s="7">
         <v>10</v>
       </c>
       <c r="AX6" s="1">
@@ -5298,7 +5518,47 @@
       <c r="AY6" s="1">
         <v>10.31</v>
       </c>
-      <c r="CO6" s="6">
+      <c r="BA6" s="7">
+        <v>40</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BG6" s="7">
+        <v>10</v>
+      </c>
+      <c r="BH6" s="1">
+        <v>46</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>9.24</v>
+      </c>
+      <c r="BK6" s="7">
+        <v>40</v>
+      </c>
+      <c r="BL6" s="1"/>
+      <c r="BM6" s="1"/>
+      <c r="BN6" s="1"/>
+      <c r="BO6" s="1"/>
+      <c r="BP6" s="1"/>
+      <c r="BQ6" s="7">
+        <v>10</v>
+      </c>
+      <c r="BR6" s="1"/>
+      <c r="BS6" s="1"/>
+      <c r="CO6" s="7">
         <v>40</v>
       </c>
       <c r="CP6" s="1"/>
@@ -5306,12 +5566,12 @@
       <c r="CR6" s="1"/>
       <c r="CS6" s="1"/>
       <c r="CT6" s="1"/>
-      <c r="CU6" s="6"/>
+      <c r="CU6" s="7"/>
       <c r="CV6" s="1"/>
       <c r="CW6" s="1"/>
     </row>
     <row r="7" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="1">
         <v>0</v>
       </c>
@@ -5327,14 +5587,14 @@
       <c r="H7" s="1">
         <v>-61</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="7"/>
       <c r="J7" s="1">
         <v>29</v>
       </c>
       <c r="K7" s="1">
         <v>5.81</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="1">
         <v>0</v>
       </c>
@@ -5350,14 +5610,14 @@
       <c r="R7" s="1">
         <v>-74</v>
       </c>
-      <c r="S7" s="6"/>
+      <c r="S7" s="7"/>
       <c r="T7" s="1">
         <v>25</v>
       </c>
       <c r="U7" s="1">
         <v>5.19</v>
       </c>
-      <c r="W7" s="6"/>
+      <c r="W7" s="7"/>
       <c r="X7" s="1">
         <v>0</v>
       </c>
@@ -5373,14 +5633,14 @@
       <c r="AB7" s="1">
         <v>-40</v>
       </c>
-      <c r="AC7" s="6"/>
+      <c r="AC7" s="7"/>
       <c r="AD7" s="1">
         <v>51</v>
       </c>
       <c r="AE7" s="1">
         <v>10.33</v>
       </c>
-      <c r="AG7" s="6"/>
+      <c r="AG7" s="7"/>
       <c r="AH7" s="1">
         <v>0</v>
       </c>
@@ -5396,14 +5656,14 @@
       <c r="AL7" s="1">
         <v>-53</v>
       </c>
-      <c r="AM7" s="6"/>
+      <c r="AM7" s="7"/>
       <c r="AN7" s="1">
         <v>51</v>
       </c>
       <c r="AO7" s="1">
         <v>10.15</v>
       </c>
-      <c r="AQ7" s="6"/>
+      <c r="AQ7" s="7"/>
       <c r="AR7" s="1">
         <v>0</v>
       </c>
@@ -5419,25 +5679,57 @@
       <c r="AV7" s="1">
         <v>-53</v>
       </c>
-      <c r="AW7" s="6"/>
+      <c r="AW7" s="7"/>
       <c r="AX7" s="1">
         <v>51</v>
       </c>
       <c r="AY7" s="1">
         <v>10.35</v>
       </c>
-      <c r="CO7" s="6"/>
+      <c r="BA7" s="7"/>
+      <c r="BB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
+        <v>-47</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>-47</v>
+      </c>
+      <c r="BG7" s="7"/>
+      <c r="BH7" s="1">
+        <v>156</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>31.85</v>
+      </c>
+      <c r="BK7" s="7"/>
+      <c r="BL7" s="1"/>
+      <c r="BM7" s="1"/>
+      <c r="BN7" s="1"/>
+      <c r="BO7" s="1"/>
+      <c r="BP7" s="1"/>
+      <c r="BQ7" s="7"/>
+      <c r="BR7" s="1"/>
+      <c r="BS7" s="1"/>
+      <c r="CO7" s="7"/>
       <c r="CP7" s="1"/>
       <c r="CQ7" s="1"/>
       <c r="CR7" s="1"/>
       <c r="CS7" s="1"/>
       <c r="CT7" s="1"/>
-      <c r="CU7" s="6"/>
+      <c r="CU7" s="7"/>
       <c r="CV7" s="1"/>
       <c r="CW7" s="1"/>
     </row>
     <row r="8" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" s="1">
         <v>0</v>
       </c>
@@ -5453,14 +5745,14 @@
       <c r="H8" s="1">
         <v>-57</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="1">
         <v>29</v>
       </c>
       <c r="K8" s="1">
         <v>5.8</v>
       </c>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7"/>
       <c r="N8" s="1">
         <v>0</v>
       </c>
@@ -5476,14 +5768,14 @@
       <c r="R8" s="1">
         <v>-73</v>
       </c>
-      <c r="S8" s="6"/>
+      <c r="S8" s="7"/>
       <c r="T8" s="1">
         <v>27</v>
       </c>
       <c r="U8" s="1">
         <v>5.45</v>
       </c>
-      <c r="W8" s="6"/>
+      <c r="W8" s="7"/>
       <c r="X8" s="1">
         <v>0</v>
       </c>
@@ -5499,14 +5791,14 @@
       <c r="AB8" s="1">
         <v>-42</v>
       </c>
-      <c r="AC8" s="6"/>
+      <c r="AC8" s="7"/>
       <c r="AD8" s="1">
         <v>51</v>
       </c>
       <c r="AE8" s="1">
         <v>10.199999999999999</v>
       </c>
-      <c r="AG8" s="6"/>
+      <c r="AG8" s="7"/>
       <c r="AH8" s="1">
         <v>0</v>
       </c>
@@ -5522,14 +5814,14 @@
       <c r="AL8" s="1">
         <v>-54</v>
       </c>
-      <c r="AM8" s="6"/>
+      <c r="AM8" s="7"/>
       <c r="AN8" s="1">
         <v>51</v>
       </c>
       <c r="AO8" s="1">
         <v>9.24</v>
       </c>
-      <c r="AQ8" s="6"/>
+      <c r="AQ8" s="7"/>
       <c r="AR8" s="1">
         <v>0</v>
       </c>
@@ -5545,25 +5837,57 @@
       <c r="AV8" s="1">
         <v>-52</v>
       </c>
-      <c r="AW8" s="6"/>
+      <c r="AW8" s="7"/>
       <c r="AX8" s="1">
         <v>51</v>
       </c>
       <c r="AY8" s="1">
         <v>10.14</v>
       </c>
-      <c r="CO8" s="6"/>
+      <c r="BA8" s="7"/>
+      <c r="BB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>-49</v>
+      </c>
+      <c r="BG8" s="7"/>
+      <c r="BH8" s="1">
+        <v>147</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>30.05</v>
+      </c>
+      <c r="BK8" s="7"/>
+      <c r="BL8" s="1"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="7"/>
+      <c r="BR8" s="1"/>
+      <c r="BS8" s="1"/>
+      <c r="CO8" s="7"/>
       <c r="CP8" s="1"/>
       <c r="CQ8" s="1"/>
       <c r="CR8" s="1"/>
       <c r="CS8" s="1"/>
       <c r="CT8" s="1"/>
-      <c r="CU8" s="6"/>
+      <c r="CU8" s="7"/>
       <c r="CV8" s="1"/>
       <c r="CW8" s="1"/>
     </row>
     <row r="9" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="1">
         <v>0</v>
       </c>
@@ -5579,14 +5903,14 @@
       <c r="H9" s="1">
         <v>-62</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="1">
         <v>29</v>
       </c>
       <c r="K9" s="1">
         <v>5.78</v>
       </c>
-      <c r="M9" s="6"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="1">
         <v>0</v>
       </c>
@@ -5602,14 +5926,14 @@
       <c r="R9" s="1">
         <v>-76</v>
       </c>
-      <c r="S9" s="6"/>
+      <c r="S9" s="7"/>
       <c r="T9" s="1">
         <v>26</v>
       </c>
       <c r="U9" s="1">
         <v>5.15</v>
       </c>
-      <c r="W9" s="6"/>
+      <c r="W9" s="7"/>
       <c r="X9" s="1">
         <v>0</v>
       </c>
@@ -5625,14 +5949,14 @@
       <c r="AB9" s="1">
         <v>-41</v>
       </c>
-      <c r="AC9" s="6"/>
+      <c r="AC9" s="7"/>
       <c r="AD9" s="1">
         <v>51</v>
       </c>
       <c r="AE9" s="1">
         <v>10.130000000000001</v>
       </c>
-      <c r="AG9" s="6"/>
+      <c r="AG9" s="7"/>
       <c r="AH9" s="1">
         <v>0</v>
       </c>
@@ -5648,14 +5972,14 @@
       <c r="AL9" s="1">
         <v>-54</v>
       </c>
-      <c r="AM9" s="6"/>
+      <c r="AM9" s="7"/>
       <c r="AN9" s="1">
         <v>51</v>
       </c>
       <c r="AO9" s="1">
         <v>8.7100000000000009</v>
       </c>
-      <c r="AQ9" s="6"/>
+      <c r="AQ9" s="7"/>
       <c r="AR9" s="1">
         <v>0</v>
       </c>
@@ -5671,25 +5995,57 @@
       <c r="AV9" s="1">
         <v>-47</v>
       </c>
-      <c r="AW9" s="6"/>
+      <c r="AW9" s="7"/>
       <c r="AX9" s="1">
         <v>51</v>
       </c>
       <c r="AY9" s="1">
         <v>8.8699999999999992</v>
       </c>
-      <c r="CO9" s="6"/>
+      <c r="BA9" s="7"/>
+      <c r="BB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BF9" s="1">
+        <v>-50</v>
+      </c>
+      <c r="BG9" s="7"/>
+      <c r="BH9" s="1">
+        <v>144</v>
+      </c>
+      <c r="BI9" s="1">
+        <v>29.39</v>
+      </c>
+      <c r="BK9" s="7"/>
+      <c r="BL9" s="1"/>
+      <c r="BM9" s="1"/>
+      <c r="BN9" s="1"/>
+      <c r="BO9" s="1"/>
+      <c r="BP9" s="1"/>
+      <c r="BQ9" s="7"/>
+      <c r="BR9" s="1"/>
+      <c r="BS9" s="1"/>
+      <c r="CO9" s="7"/>
       <c r="CP9" s="1"/>
       <c r="CQ9" s="1"/>
       <c r="CR9" s="1"/>
       <c r="CS9" s="1"/>
       <c r="CT9" s="1"/>
-      <c r="CU9" s="6"/>
+      <c r="CU9" s="7"/>
       <c r="CV9" s="1"/>
       <c r="CW9" s="1"/>
     </row>
     <row r="10" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" s="1">
         <v>0</v>
       </c>
@@ -5705,14 +6061,14 @@
       <c r="H10" s="1">
         <v>-57</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="1">
         <v>29</v>
       </c>
       <c r="K10" s="1">
         <v>5.79</v>
       </c>
-      <c r="M10" s="6"/>
+      <c r="M10" s="7"/>
       <c r="N10" s="1">
         <v>0</v>
       </c>
@@ -5728,14 +6084,14 @@
       <c r="R10" s="1">
         <v>-80</v>
       </c>
-      <c r="S10" s="6"/>
+      <c r="S10" s="7"/>
       <c r="T10" s="1">
         <v>25</v>
       </c>
       <c r="U10" s="1">
         <v>4.96</v>
       </c>
-      <c r="W10" s="6"/>
+      <c r="W10" s="7"/>
       <c r="X10" s="1">
         <v>0</v>
       </c>
@@ -5751,14 +6107,14 @@
       <c r="AB10" s="1">
         <v>-41</v>
       </c>
-      <c r="AC10" s="6"/>
+      <c r="AC10" s="7"/>
       <c r="AD10" s="1">
         <v>51</v>
       </c>
       <c r="AE10" s="1">
         <v>10.19</v>
       </c>
-      <c r="AG10" s="6"/>
+      <c r="AG10" s="7"/>
       <c r="AH10" s="1">
         <v>0</v>
       </c>
@@ -5774,14 +6130,14 @@
       <c r="AL10" s="1">
         <v>-53</v>
       </c>
-      <c r="AM10" s="6"/>
+      <c r="AM10" s="7"/>
       <c r="AN10" s="1">
         <v>51</v>
       </c>
       <c r="AO10" s="1">
         <v>9.43</v>
       </c>
-      <c r="AQ10" s="6"/>
+      <c r="AQ10" s="7"/>
       <c r="AR10" s="1">
         <v>0</v>
       </c>
@@ -5797,20 +6153,52 @@
       <c r="AV10" s="1">
         <v>-55</v>
       </c>
-      <c r="AW10" s="6"/>
+      <c r="AW10" s="7"/>
       <c r="AX10" s="1">
         <v>50</v>
       </c>
       <c r="AY10" s="1">
         <v>10.16</v>
       </c>
-      <c r="CO10" s="6"/>
+      <c r="BA10" s="7"/>
+      <c r="BB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE10" s="1">
+        <v>-49</v>
+      </c>
+      <c r="BF10" s="1">
+        <v>-49</v>
+      </c>
+      <c r="BG10" s="7"/>
+      <c r="BH10" s="1">
+        <v>151</v>
+      </c>
+      <c r="BI10" s="1">
+        <v>30.85</v>
+      </c>
+      <c r="BK10" s="7"/>
+      <c r="BL10" s="1"/>
+      <c r="BM10" s="1"/>
+      <c r="BN10" s="1"/>
+      <c r="BO10" s="1"/>
+      <c r="BP10" s="1"/>
+      <c r="BQ10" s="7"/>
+      <c r="BR10" s="1"/>
+      <c r="BS10" s="1"/>
+      <c r="CO10" s="7"/>
       <c r="CP10" s="1"/>
       <c r="CQ10" s="1"/>
       <c r="CR10" s="1"/>
       <c r="CS10" s="1"/>
       <c r="CT10" s="1"/>
-      <c r="CU10" s="6"/>
+      <c r="CU10" s="7"/>
       <c r="CV10" s="1"/>
       <c r="CW10" s="1"/>
     </row>
@@ -5985,6 +6373,74 @@
         <f t="shared" si="10"/>
         <v>9.9659999999999993</v>
       </c>
+      <c r="BA11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB11" s="6">
+        <f>SUM(BB6:BB10)/(5-COUNTBLANK(BB6:BB10))</f>
+        <v>0</v>
+      </c>
+      <c r="BC11" s="6">
+        <f t="shared" ref="BC11:BF11" si="11">SUM(BC6:BC10)/(5-COUNTBLANK(BC6:BC10))</f>
+        <v>40</v>
+      </c>
+      <c r="BD11" s="6">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BE11" s="6">
+        <f t="shared" si="11"/>
+        <v>-46.8</v>
+      </c>
+      <c r="BF11" s="6">
+        <f t="shared" si="11"/>
+        <v>-48.2</v>
+      </c>
+      <c r="BG11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH11" s="6">
+        <f t="shared" ref="BH11:BI11" si="12">SUM(BH6:BH10)/(5-COUNTBLANK(BH6:BH10))</f>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="BI11" s="6">
+        <f t="shared" si="12"/>
+        <v>26.276</v>
+      </c>
+      <c r="BK11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BL11" s="6" t="e">
+        <f>SUM(BL6:BL10)/(5-COUNTBLANK(BL6:BL10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BM11" s="6" t="e">
+        <f t="shared" ref="BM11:BP11" si="13">SUM(BM6:BM10)/(5-COUNTBLANK(BM6:BM10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BN11" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BO11" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BP11" s="6" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BQ11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR11" s="6" t="e">
+        <f t="shared" ref="BR11:BS11" si="14">SUM(BR6:BR10)/(5-COUNTBLANK(BR6:BR10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BS11" s="6" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="CO11" s="4" t="s">
         <v>15</v>
       </c>
@@ -5993,42 +6449,42 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CQ11" s="4" t="e">
-        <f t="shared" ref="CQ11:CT11" si="11">SUM(CQ6:CQ10)/(5-COUNTBLANK(CQ6:CQ10))</f>
+        <f t="shared" ref="CQ11:CT11" si="15">SUM(CQ6:CQ10)/(5-COUNTBLANK(CQ6:CQ10))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="CR11" s="4" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CS11" s="4" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CT11" s="4" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CU11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="CV11" s="4" t="e">
-        <f t="shared" ref="CV11:CW11" si="12">SUM(CV6:CV10)/(5-COUNTBLANK(CV6:CV10))</f>
+        <f t="shared" ref="CV11:CW11" si="16">SUM(CV6:CV10)/(5-COUNTBLANK(CV6:CV10))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="CW11" s="4" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="12"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="2:101" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
@@ -6052,31 +6508,64 @@
       <c r="I14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W14" s="8" t="s">
+      <c r="W14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AG14" s="8" t="s">
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AG14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="AH14" s="8"/>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="8"/>
-      <c r="AO14" s="8"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
+      <c r="AN14" s="9"/>
+      <c r="AO14" s="9"/>
+      <c r="AQ14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AR14" s="9"/>
+      <c r="AS14" s="9"/>
+      <c r="AT14" s="9"/>
+      <c r="AU14" s="9"/>
+      <c r="AV14" s="9"/>
+      <c r="AW14" s="9"/>
+      <c r="AX14" s="9"/>
+      <c r="AY14" s="9"/>
+      <c r="BA14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB14" s="9"/>
+      <c r="BC14" s="9"/>
+      <c r="BD14" s="9"/>
+      <c r="BE14" s="9"/>
+      <c r="BF14" s="9"/>
+      <c r="BG14" s="9"/>
+      <c r="BH14" s="9"/>
+      <c r="BI14" s="9"/>
+      <c r="BK14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="BL14" s="9"/>
+      <c r="BM14" s="9"/>
+      <c r="BN14" s="9"/>
+      <c r="BO14" s="9"/>
+      <c r="BP14" s="9"/>
+      <c r="BQ14" s="9"/>
+      <c r="BR14" s="9"/>
+      <c r="BS14" s="9"/>
     </row>
     <row r="15" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -6106,35 +6595,74 @@
         <f>K11</f>
         <v>5.798</v>
       </c>
-      <c r="W15" s="7" t="s">
+      <c r="W15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="8" t="s">
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AG15" s="7" t="s">
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AG15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AH15" s="7"/>
-      <c r="AI15" s="7"/>
-      <c r="AJ15" s="7"/>
-      <c r="AK15" s="7"/>
-      <c r="AL15" s="7"/>
-      <c r="AM15" s="8" t="s">
+      <c r="AH15" s="8"/>
+      <c r="AI15" s="8"/>
+      <c r="AJ15" s="8"/>
+      <c r="AK15" s="8"/>
+      <c r="AL15" s="8"/>
+      <c r="AM15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="8"/>
+      <c r="AN15" s="9"/>
+      <c r="AO15" s="9"/>
+      <c r="AQ15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR15" s="8"/>
+      <c r="AS15" s="8"/>
+      <c r="AT15" s="8"/>
+      <c r="AU15" s="8"/>
+      <c r="AV15" s="8"/>
+      <c r="AW15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX15" s="9"/>
+      <c r="AY15" s="9"/>
+      <c r="BA15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB15" s="8"/>
+      <c r="BC15" s="8"/>
+      <c r="BD15" s="8"/>
+      <c r="BE15" s="8"/>
+      <c r="BF15" s="8"/>
+      <c r="BG15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH15" s="9"/>
+      <c r="BI15" s="9"/>
+      <c r="BK15" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL15" s="8"/>
+      <c r="BM15" s="8"/>
+      <c r="BN15" s="8"/>
+      <c r="BO15" s="8"/>
+      <c r="BP15" s="8"/>
+      <c r="BQ15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR15" s="9"/>
+      <c r="BS15" s="9"/>
     </row>
     <row r="16" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B16" s="14"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="1" t="s">
         <v>21</v>
       </c>
@@ -6162,59 +6690,134 @@
         <f>U11</f>
         <v>5.19</v>
       </c>
-      <c r="W16" s="7" t="s">
+      <c r="W16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="X16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="7" t="s">
+      <c r="X16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Z16" s="7" t="s">
+      <c r="Z16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AA16" s="8" t="s">
+      <c r="AA16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="7" t="s">
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AD16" s="7" t="s">
+      <c r="AD16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AE16" s="7" t="s">
+      <c r="AE16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AG16" s="7" t="s">
+      <c r="AG16" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AH16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="7" t="s">
+      <c r="AH16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AJ16" s="7" t="s">
+      <c r="AJ16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AK16" s="8" t="s">
+      <c r="AK16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="7" t="s">
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AN16" s="7" t="s">
+      <c r="AN16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AO16" s="7" t="s">
+      <c r="AO16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV16" s="9"/>
+      <c r="AW16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF16" s="9"/>
+      <c r="BG16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BH16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP16" s="9"/>
+      <c r="BQ16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS16" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:92" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -6244,48 +6847,87 @@
         <f>AE11</f>
         <v>10.225999999999999</v>
       </c>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
-      <c r="Z17" s="7"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
       <c r="AA17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="7"/>
-      <c r="AE17" s="7"/>
-      <c r="AG17" s="7"/>
-      <c r="AH17" s="7"/>
-      <c r="AI17" s="7"/>
-      <c r="AJ17" s="7"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
       <c r="AK17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AL17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AM17" s="7"/>
-      <c r="AN17" s="7"/>
-      <c r="AO17" s="7"/>
-      <c r="CF17" s="7" t="s">
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="8"/>
+      <c r="AO17" s="8"/>
+      <c r="AQ17" s="8"/>
+      <c r="AR17" s="8"/>
+      <c r="AS17" s="8"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW17" s="8"/>
+      <c r="AX17" s="8"/>
+      <c r="AY17" s="8"/>
+      <c r="BA17" s="8"/>
+      <c r="BB17" s="8"/>
+      <c r="BC17" s="8"/>
+      <c r="BD17" s="8"/>
+      <c r="BE17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG17" s="8"/>
+      <c r="BH17" s="8"/>
+      <c r="BI17" s="8"/>
+      <c r="BK17" s="8"/>
+      <c r="BL17" s="8"/>
+      <c r="BM17" s="8"/>
+      <c r="BN17" s="8"/>
+      <c r="BO17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BP17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ17" s="8"/>
+      <c r="BR17" s="8"/>
+      <c r="BS17" s="8"/>
+      <c r="CF17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="CG17" s="7"/>
-      <c r="CH17" s="7"/>
-      <c r="CI17" s="7"/>
-      <c r="CJ17" s="7"/>
-      <c r="CK17" s="7"/>
-      <c r="CL17" s="8" t="s">
+      <c r="CG17" s="8"/>
+      <c r="CH17" s="8"/>
+      <c r="CI17" s="8"/>
+      <c r="CJ17" s="8"/>
+      <c r="CK17" s="8"/>
+      <c r="CL17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="CM17" s="8"/>
-      <c r="CN17" s="8"/>
+      <c r="CM17" s="9"/>
+      <c r="CN17" s="9"/>
     </row>
     <row r="18" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="B18" s="10"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
@@ -6313,7 +6955,7 @@
         <f>AE23</f>
         <v>10.306000000000001</v>
       </c>
-      <c r="W18" s="6">
+      <c r="W18" s="7">
         <v>40</v>
       </c>
       <c r="X18" s="1">
@@ -6331,7 +6973,7 @@
       <c r="AB18" s="1">
         <v>-40</v>
       </c>
-      <c r="AC18" s="6">
+      <c r="AC18" s="7">
         <v>10</v>
       </c>
       <c r="AD18" s="1">
@@ -6340,7 +6982,7 @@
       <c r="AE18" s="1">
         <v>10.37</v>
       </c>
-      <c r="AG18" s="6">
+      <c r="AG18" s="7">
         <v>40</v>
       </c>
       <c r="AH18" s="1">
@@ -6358,7 +7000,7 @@
       <c r="AL18" s="1">
         <v>-52</v>
       </c>
-      <c r="AM18" s="6">
+      <c r="AM18" s="7">
         <v>10</v>
       </c>
       <c r="AN18" s="1">
@@ -6367,34 +7009,101 @@
       <c r="AO18" s="1">
         <v>10.3</v>
       </c>
-      <c r="CF18" s="7" t="s">
+      <c r="AQ18" s="7">
+        <v>40</v>
+      </c>
+      <c r="AR18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="1">
+        <v>-55</v>
+      </c>
+      <c r="AV18" s="1">
+        <v>-57</v>
+      </c>
+      <c r="AW18" s="7">
+        <v>10</v>
+      </c>
+      <c r="AX18" s="1">
+        <v>64</v>
+      </c>
+      <c r="AY18" s="1">
+        <v>12.57</v>
+      </c>
+      <c r="BA18" s="7">
+        <v>40</v>
+      </c>
+      <c r="BB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC18" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE18" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BF18" s="1">
+        <v>-49</v>
+      </c>
+      <c r="BG18" s="7">
+        <v>10</v>
+      </c>
+      <c r="BH18" s="1">
+        <v>164</v>
+      </c>
+      <c r="BI18" s="1">
+        <v>33.549999999999997</v>
+      </c>
+      <c r="BK18" s="7">
+        <v>40</v>
+      </c>
+      <c r="BL18" s="1"/>
+      <c r="BM18" s="1"/>
+      <c r="BN18" s="1"/>
+      <c r="BO18" s="1"/>
+      <c r="BP18" s="1"/>
+      <c r="BQ18" s="7">
+        <v>10</v>
+      </c>
+      <c r="BR18" s="1"/>
+      <c r="BS18" s="1"/>
+      <c r="CF18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="CG18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="CH18" s="7" t="s">
+      <c r="CG18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="CH18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="CI18" s="7" t="s">
+      <c r="CI18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="CJ18" s="8" t="s">
+      <c r="CJ18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="CK18" s="8"/>
-      <c r="CL18" s="7" t="s">
+      <c r="CK18" s="9"/>
+      <c r="CL18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="CM18" s="7" t="s">
+      <c r="CM18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="CN18" s="7" t="s">
+      <c r="CN18" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="B19" s="10"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="1" t="s">
         <v>29</v>
       </c>
@@ -6422,7 +7131,7 @@
         <f>AE35</f>
         <v>9.9280000000000008</v>
       </c>
-      <c r="W19" s="6"/>
+      <c r="W19" s="7"/>
       <c r="X19" s="1">
         <v>0</v>
       </c>
@@ -6438,14 +7147,14 @@
       <c r="AB19" s="1">
         <v>-40</v>
       </c>
-      <c r="AC19" s="6"/>
+      <c r="AC19" s="7"/>
       <c r="AD19" s="1">
         <v>51</v>
       </c>
       <c r="AE19" s="1">
         <v>10.39</v>
       </c>
-      <c r="AG19" s="6"/>
+      <c r="AG19" s="7"/>
       <c r="AH19" s="1">
         <v>0</v>
       </c>
@@ -6461,29 +7170,84 @@
       <c r="AL19" s="1">
         <v>-58</v>
       </c>
-      <c r="AM19" s="6"/>
+      <c r="AM19" s="7"/>
       <c r="AN19" s="1">
         <v>51</v>
       </c>
       <c r="AO19" s="1">
         <v>10.34</v>
       </c>
-      <c r="CF19" s="7"/>
-      <c r="CG19" s="7"/>
-      <c r="CH19" s="7"/>
-      <c r="CI19" s="7"/>
+      <c r="AQ19" s="7"/>
+      <c r="AR19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="1">
+        <v>-59</v>
+      </c>
+      <c r="AV19" s="1">
+        <v>-63</v>
+      </c>
+      <c r="AW19" s="7"/>
+      <c r="AX19" s="1">
+        <v>95</v>
+      </c>
+      <c r="AY19" s="1">
+        <v>19.309999999999999</v>
+      </c>
+      <c r="BA19" s="7"/>
+      <c r="BB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC19" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE19" s="1">
+        <v>-47</v>
+      </c>
+      <c r="BF19" s="1">
+        <v>-48</v>
+      </c>
+      <c r="BG19" s="7"/>
+      <c r="BH19" s="1">
+        <v>163</v>
+      </c>
+      <c r="BI19" s="1">
+        <v>33.26</v>
+      </c>
+      <c r="BK19" s="7"/>
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="1"/>
+      <c r="BN19" s="1"/>
+      <c r="BO19" s="1"/>
+      <c r="BP19" s="1"/>
+      <c r="BQ19" s="7"/>
+      <c r="BR19" s="1"/>
+      <c r="BS19" s="1"/>
+      <c r="CF19" s="8"/>
+      <c r="CG19" s="8"/>
+      <c r="CH19" s="8"/>
+      <c r="CI19" s="8"/>
       <c r="CJ19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="CK19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="CL19" s="7"/>
-      <c r="CM19" s="7"/>
-      <c r="CN19" s="7"/>
+      <c r="CL19" s="8"/>
+      <c r="CM19" s="8"/>
+      <c r="CN19" s="8"/>
     </row>
     <row r="20" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="B20" s="10"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="1" t="s">
         <v>30</v>
       </c>
@@ -6511,7 +7275,7 @@
         <f>AO11</f>
         <v>9.5860000000000003</v>
       </c>
-      <c r="W20" s="6"/>
+      <c r="W20" s="7"/>
       <c r="X20" s="1">
         <v>0</v>
       </c>
@@ -6527,14 +7291,14 @@
       <c r="AB20" s="1">
         <v>-40</v>
       </c>
-      <c r="AC20" s="6"/>
+      <c r="AC20" s="7"/>
       <c r="AD20" s="1">
         <v>51</v>
       </c>
       <c r="AE20" s="1">
         <v>10.29</v>
       </c>
-      <c r="AG20" s="6"/>
+      <c r="AG20" s="7"/>
       <c r="AH20" s="1">
         <v>0</v>
       </c>
@@ -6550,17 +7314,72 @@
       <c r="AL20" s="1">
         <v>-54</v>
       </c>
-      <c r="AM20" s="6"/>
+      <c r="AM20" s="7"/>
       <c r="AN20" s="1">
         <v>51</v>
       </c>
       <c r="AO20" s="1">
         <v>10.19</v>
       </c>
+      <c r="AQ20" s="7"/>
+      <c r="AR20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="1">
+        <v>-57</v>
+      </c>
+      <c r="AV20" s="1">
+        <v>-58</v>
+      </c>
+      <c r="AW20" s="7"/>
+      <c r="AX20" s="1">
+        <v>63</v>
+      </c>
+      <c r="AY20" s="1">
+        <v>12.77</v>
+      </c>
+      <c r="BA20" s="7"/>
+      <c r="BB20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE20" s="1">
+        <v>-45</v>
+      </c>
+      <c r="BF20" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BG20" s="7"/>
+      <c r="BH20" s="1">
+        <v>152</v>
+      </c>
+      <c r="BI20" s="1">
+        <v>31.08</v>
+      </c>
+      <c r="BK20" s="7"/>
+      <c r="BL20" s="1"/>
+      <c r="BM20" s="1"/>
+      <c r="BN20" s="1"/>
+      <c r="BO20" s="1"/>
+      <c r="BP20" s="1"/>
+      <c r="BQ20" s="7"/>
+      <c r="BR20" s="1"/>
+      <c r="BS20" s="1"/>
       <c r="CE20">
         <v>515</v>
       </c>
-      <c r="CF20" s="6">
+      <c r="CF20" s="7">
         <v>10</v>
       </c>
       <c r="CG20" s="1">
@@ -6578,12 +7397,12 @@
       <c r="CK20" s="1">
         <v>-60</v>
       </c>
-      <c r="CL20" s="6"/>
+      <c r="CL20" s="7"/>
       <c r="CM20" s="1"/>
       <c r="CN20" s="1"/>
     </row>
     <row r="21" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
@@ -6611,7 +7430,7 @@
         <f>AO23</f>
         <v>10.005999999999998</v>
       </c>
-      <c r="W21" s="6"/>
+      <c r="W21" s="7"/>
       <c r="X21" s="1">
         <v>0</v>
       </c>
@@ -6627,14 +7446,14 @@
       <c r="AB21" s="1">
         <v>-41</v>
       </c>
-      <c r="AC21" s="6"/>
+      <c r="AC21" s="7"/>
       <c r="AD21" s="1">
         <v>51</v>
       </c>
       <c r="AE21" s="1">
         <v>10.25</v>
       </c>
-      <c r="AG21" s="6"/>
+      <c r="AG21" s="7"/>
       <c r="AH21" s="1">
         <v>0</v>
       </c>
@@ -6650,17 +7469,72 @@
       <c r="AL21" s="1">
         <v>-57</v>
       </c>
-      <c r="AM21" s="6"/>
+      <c r="AM21" s="7"/>
       <c r="AN21" s="1">
         <v>51</v>
       </c>
       <c r="AO21" s="1">
         <v>8.8699999999999992</v>
       </c>
+      <c r="AQ21" s="7"/>
+      <c r="AR21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS21" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT21" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU21" s="1">
+        <v>-56</v>
+      </c>
+      <c r="AV21" s="1">
+        <v>-58</v>
+      </c>
+      <c r="AW21" s="7"/>
+      <c r="AX21" s="1">
+        <v>63</v>
+      </c>
+      <c r="AY21" s="1">
+        <v>12.73</v>
+      </c>
+      <c r="BA21" s="7"/>
+      <c r="BB21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC21" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD21" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE21" s="1">
+        <v>-46</v>
+      </c>
+      <c r="BF21" s="1">
+        <v>-49</v>
+      </c>
+      <c r="BG21" s="7"/>
+      <c r="BH21" s="1">
+        <v>158</v>
+      </c>
+      <c r="BI21" s="1">
+        <v>32.06</v>
+      </c>
+      <c r="BK21" s="7"/>
+      <c r="BL21" s="1"/>
+      <c r="BM21" s="1"/>
+      <c r="BN21" s="1"/>
+      <c r="BO21" s="1"/>
+      <c r="BP21" s="1"/>
+      <c r="BQ21" s="7"/>
+      <c r="BR21" s="1"/>
+      <c r="BS21" s="1"/>
       <c r="CE21">
         <v>610</v>
       </c>
-      <c r="CF21" s="6"/>
+      <c r="CF21" s="7"/>
       <c r="CG21" s="1">
         <v>0</v>
       </c>
@@ -6676,12 +7550,12 @@
       <c r="CK21" s="1">
         <v>-62</v>
       </c>
-      <c r="CL21" s="6"/>
+      <c r="CL21" s="7"/>
       <c r="CM21" s="1"/>
       <c r="CN21" s="1"/>
     </row>
     <row r="22" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="1" t="s">
         <v>32</v>
       </c>
@@ -6709,7 +7583,7 @@
         <f>AO35</f>
         <v>9.7620000000000005</v>
       </c>
-      <c r="W22" s="6"/>
+      <c r="W22" s="7"/>
       <c r="X22" s="1">
         <v>0</v>
       </c>
@@ -6725,14 +7599,14 @@
       <c r="AB22" s="1">
         <v>-40</v>
       </c>
-      <c r="AC22" s="6"/>
+      <c r="AC22" s="7"/>
       <c r="AD22" s="1">
         <v>51</v>
       </c>
       <c r="AE22" s="1">
         <v>10.23</v>
       </c>
-      <c r="AG22" s="6"/>
+      <c r="AG22" s="7"/>
       <c r="AH22" s="1">
         <v>0</v>
       </c>
@@ -6748,25 +7622,80 @@
       <c r="AL22" s="1">
         <v>-58</v>
       </c>
-      <c r="AM22" s="6"/>
+      <c r="AM22" s="7"/>
       <c r="AN22" s="1">
         <v>51</v>
       </c>
       <c r="AO22" s="1">
         <v>10.33</v>
       </c>
-      <c r="CF22" s="6"/>
+      <c r="AQ22" s="7"/>
+      <c r="AR22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS22" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT22" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU22" s="1">
+        <v>-57</v>
+      </c>
+      <c r="AV22" s="1">
+        <v>-56</v>
+      </c>
+      <c r="AW22" s="7"/>
+      <c r="AX22" s="1">
+        <v>63</v>
+      </c>
+      <c r="AY22" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="BA22" s="7"/>
+      <c r="BB22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC22" s="1">
+        <v>40</v>
+      </c>
+      <c r="BD22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE22" s="1">
+        <v>-48</v>
+      </c>
+      <c r="BF22" s="1">
+        <v>-48</v>
+      </c>
+      <c r="BG22" s="7"/>
+      <c r="BH22" s="1">
+        <v>160</v>
+      </c>
+      <c r="BI22" s="1">
+        <v>32.520000000000003</v>
+      </c>
+      <c r="BK22" s="7"/>
+      <c r="BL22" s="1"/>
+      <c r="BM22" s="1"/>
+      <c r="BN22" s="1"/>
+      <c r="BO22" s="1"/>
+      <c r="BP22" s="1"/>
+      <c r="BQ22" s="7"/>
+      <c r="BR22" s="1"/>
+      <c r="BS22" s="1"/>
+      <c r="CF22" s="7"/>
       <c r="CG22" s="1"/>
       <c r="CH22" s="1"/>
       <c r="CI22" s="1"/>
       <c r="CJ22" s="1"/>
       <c r="CK22" s="1"/>
-      <c r="CL22" s="6"/>
+      <c r="CL22" s="7"/>
       <c r="CM22" s="1"/>
       <c r="CN22" s="1"/>
     </row>
     <row r="23" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="5" t="s">
         <v>36</v>
       </c>
@@ -6802,30 +7731,30 @@
         <v>0</v>
       </c>
       <c r="Y23" s="2">
-        <f t="shared" ref="Y23" si="13">SUM(Y18:Y22)/(5-COUNTBLANK(Y18:Y22))</f>
+        <f t="shared" ref="Y23" si="17">SUM(Y18:Y22)/(5-COUNTBLANK(Y18:Y22))</f>
         <v>40</v>
       </c>
       <c r="Z23" s="2">
-        <f t="shared" ref="Z23" si="14">SUM(Z18:Z22)/(5-COUNTBLANK(Z18:Z22))</f>
+        <f t="shared" ref="Z23" si="18">SUM(Z18:Z22)/(5-COUNTBLANK(Z18:Z22))</f>
         <v>0</v>
       </c>
       <c r="AA23" s="2">
-        <f t="shared" ref="AA23" si="15">SUM(AA18:AA22)/(5-COUNTBLANK(AA18:AA22))</f>
+        <f t="shared" ref="AA23" si="19">SUM(AA18:AA22)/(5-COUNTBLANK(AA18:AA22))</f>
         <v>-40</v>
       </c>
       <c r="AB23" s="2">
-        <f t="shared" ref="AB23" si="16">SUM(AB18:AB22)/(5-COUNTBLANK(AB18:AB22))</f>
+        <f t="shared" ref="AB23" si="20">SUM(AB18:AB22)/(5-COUNTBLANK(AB18:AB22))</f>
         <v>-40.200000000000003</v>
       </c>
       <c r="AC23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="AD23" s="2">
-        <f t="shared" ref="AD23" si="17">SUM(AD18:AD22)/(5-COUNTBLANK(AD18:AD22))</f>
+        <f t="shared" ref="AD23" si="21">SUM(AD18:AD22)/(5-COUNTBLANK(AD18:AD22))</f>
         <v>51</v>
       </c>
       <c r="AE23" s="2">
-        <f t="shared" ref="AE23" si="18">SUM(AE18:AE22)/(5-COUNTBLANK(AE18:AE22))</f>
+        <f t="shared" ref="AE23" si="22">SUM(AE18:AE22)/(5-COUNTBLANK(AE18:AE22))</f>
         <v>10.306000000000001</v>
       </c>
       <c r="AG23" s="2" t="s">
@@ -6836,54 +7765,212 @@
         <v>0</v>
       </c>
       <c r="AI23" s="2">
-        <f t="shared" ref="AI23" si="19">SUM(AI18:AI22)/(5-COUNTBLANK(AI18:AI22))</f>
+        <f t="shared" ref="AI23" si="23">SUM(AI18:AI22)/(5-COUNTBLANK(AI18:AI22))</f>
         <v>40</v>
       </c>
       <c r="AJ23" s="2">
-        <f t="shared" ref="AJ23" si="20">SUM(AJ18:AJ22)/(5-COUNTBLANK(AJ18:AJ22))</f>
+        <f t="shared" ref="AJ23" si="24">SUM(AJ18:AJ22)/(5-COUNTBLANK(AJ18:AJ22))</f>
         <v>0</v>
       </c>
       <c r="AK23" s="2">
-        <f t="shared" ref="AK23" si="21">SUM(AK18:AK22)/(5-COUNTBLANK(AK18:AK22))</f>
+        <f t="shared" ref="AK23" si="25">SUM(AK18:AK22)/(5-COUNTBLANK(AK18:AK22))</f>
         <v>-53.2</v>
       </c>
       <c r="AL23" s="2">
-        <f t="shared" ref="AL23" si="22">SUM(AL18:AL22)/(5-COUNTBLANK(AL18:AL22))</f>
+        <f t="shared" ref="AL23" si="26">SUM(AL18:AL22)/(5-COUNTBLANK(AL18:AL22))</f>
         <v>-55.8</v>
       </c>
       <c r="AM23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="AN23" s="2">
-        <f t="shared" ref="AN23" si="23">SUM(AN18:AN22)/(5-COUNTBLANK(AN18:AN22))</f>
+        <f t="shared" ref="AN23" si="27">SUM(AN18:AN22)/(5-COUNTBLANK(AN18:AN22))</f>
         <v>51</v>
       </c>
       <c r="AO23" s="2">
-        <f t="shared" ref="AO23" si="24">SUM(AO18:AO22)/(5-COUNTBLANK(AO18:AO22))</f>
+        <f t="shared" ref="AO23" si="28">SUM(AO18:AO22)/(5-COUNTBLANK(AO18:AO22))</f>
         <v>10.005999999999998</v>
       </c>
-      <c r="CF23" s="6"/>
+      <c r="AQ23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR23" s="6">
+        <f>SUM(AR18:AR22)/(5-COUNTBLANK(AR18:AR22))</f>
+        <v>0</v>
+      </c>
+      <c r="AS23" s="6">
+        <f t="shared" ref="AS23:AV23" si="29">SUM(AS18:AS22)/(5-COUNTBLANK(AS18:AS22))</f>
+        <v>40</v>
+      </c>
+      <c r="AT23" s="6">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AU23" s="6">
+        <f t="shared" si="29"/>
+        <v>-56.8</v>
+      </c>
+      <c r="AV23" s="6">
+        <f t="shared" si="29"/>
+        <v>-58.4</v>
+      </c>
+      <c r="AW23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX23" s="6">
+        <f t="shared" ref="AX23:AY23" si="30">SUM(AX18:AX22)/(5-COUNTBLANK(AX18:AX22))</f>
+        <v>69.599999999999994</v>
+      </c>
+      <c r="AY23" s="6">
+        <f t="shared" si="30"/>
+        <v>14.916</v>
+      </c>
+      <c r="BA23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB23" s="6">
+        <f>SUM(BB18:BB22)/(5-COUNTBLANK(BB18:BB22))</f>
+        <v>0</v>
+      </c>
+      <c r="BC23" s="6">
+        <f t="shared" ref="BC23:BF23" si="31">SUM(BC18:BC22)/(5-COUNTBLANK(BC18:BC22))</f>
+        <v>40</v>
+      </c>
+      <c r="BD23" s="6">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="BE23" s="6">
+        <f t="shared" si="31"/>
+        <v>-46.4</v>
+      </c>
+      <c r="BF23" s="6">
+        <f t="shared" si="31"/>
+        <v>-48</v>
+      </c>
+      <c r="BG23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH23" s="6">
+        <f t="shared" ref="BH23:BI23" si="32">SUM(BH18:BH22)/(5-COUNTBLANK(BH18:BH22))</f>
+        <v>159.4</v>
+      </c>
+      <c r="BI23" s="6">
+        <f t="shared" si="32"/>
+        <v>32.494</v>
+      </c>
+      <c r="BK23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BL23" s="6" t="e">
+        <f>SUM(BL18:BL22)/(5-COUNTBLANK(BL18:BL22))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BM23" s="6" t="e">
+        <f t="shared" ref="BM23:BP23" si="33">SUM(BM18:BM22)/(5-COUNTBLANK(BM18:BM22))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BN23" s="6" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BO23" s="6" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BP23" s="6" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BQ23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR23" s="6" t="e">
+        <f t="shared" ref="BR23:BS23" si="34">SUM(BR18:BR22)/(5-COUNTBLANK(BR18:BR22))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BS23" s="6" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="CF23" s="7"/>
       <c r="CG23" s="1"/>
       <c r="CH23" s="1"/>
       <c r="CI23" s="1"/>
       <c r="CJ23" s="1"/>
       <c r="CK23" s="1"/>
-      <c r="CL23" s="6"/>
+      <c r="CL23" s="7"/>
       <c r="CM23" s="1"/>
       <c r="CN23" s="1"/>
     </row>
     <row r="24" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="CF24" s="6"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="3">
+        <f>AS23/AQ18</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <f>AT23</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <f>AU23</f>
+        <v>-56.8</v>
+      </c>
+      <c r="G24" s="1">
+        <f>AV23</f>
+        <v>-58.4</v>
+      </c>
+      <c r="H24" s="1">
+        <f>AX23</f>
+        <v>69.599999999999994</v>
+      </c>
+      <c r="I24" s="1">
+        <f>AY23</f>
+        <v>14.916</v>
+      </c>
+      <c r="CF24" s="7"/>
       <c r="CG24" s="1"/>
       <c r="CH24" s="1"/>
       <c r="CI24" s="1"/>
       <c r="CJ24" s="1"/>
       <c r="CK24" s="1"/>
-      <c r="CL24" s="6"/>
+      <c r="CL24" s="7"/>
       <c r="CM24" s="1"/>
       <c r="CN24" s="1"/>
     </row>
     <row r="25" spans="2:92" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
+      <c r="C25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="3">
+        <f>AS35/AQ30</f>
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <f>AT35</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <f>AU35</f>
+        <v>-53.4</v>
+      </c>
+      <c r="G25" s="1">
+        <f>AV35</f>
+        <v>-56.6</v>
+      </c>
+      <c r="H25" s="1">
+        <f>AX35</f>
+        <v>147.4</v>
+      </c>
+      <c r="I25" s="1">
+        <f>AY35</f>
+        <v>29.851999999999997</v>
+      </c>
       <c r="CF25" s="4" t="s">
         <v>15</v>
       </c>
@@ -6892,167 +7979,409 @@
         <v>0</v>
       </c>
       <c r="CH25" s="4">
-        <f t="shared" ref="CH25:CK25" si="25">SUM(CH20:CH24)/(5-COUNTBLANK(CH20:CH24))</f>
+        <f t="shared" ref="CH25:CK25" si="35">SUM(CH20:CH24)/(5-COUNTBLANK(CH20:CH24))</f>
         <v>25</v>
       </c>
       <c r="CI25" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="CJ25" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>-60</v>
       </c>
       <c r="CK25" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="35"/>
         <v>-61</v>
       </c>
       <c r="CL25" s="4" t="s">
         <v>16</v>
       </c>
       <c r="CM25" s="4" t="e">
-        <f t="shared" ref="CM25:CN25" si="26">SUM(CM20:CM24)/(5-COUNTBLANK(CM20:CM24))</f>
+        <f t="shared" ref="CM25:CN25" si="36">SUM(CM20:CM24)/(5-COUNTBLANK(CM20:CM24))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="CN25" s="4" t="e">
-        <f t="shared" si="26"/>
+        <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W26" s="8" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="3">
+        <f>BC11/BA6</f>
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <f>BD11</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <f>BE11</f>
+        <v>-46.8</v>
+      </c>
+      <c r="G26" s="1">
+        <f>BF11</f>
+        <v>-48.2</v>
+      </c>
+      <c r="H26" s="1">
+        <f>BH11</f>
+        <v>128.80000000000001</v>
+      </c>
+      <c r="I26" s="1">
+        <f>BI11</f>
+        <v>26.276</v>
+      </c>
+      <c r="W26" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8"/>
-      <c r="AB26" s="8"/>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="8"/>
-      <c r="AG26" s="8" t="s">
+      <c r="X26" s="9"/>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AG26" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AH26" s="8"/>
-      <c r="AI26" s="8"/>
-      <c r="AJ26" s="8"/>
-      <c r="AK26" s="8"/>
-      <c r="AL26" s="8"/>
-      <c r="AM26" s="8"/>
-      <c r="AN26" s="8"/>
-      <c r="AO26" s="8"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="9"/>
+      <c r="AL26" s="9"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="9"/>
+      <c r="AO26" s="9"/>
+      <c r="AQ26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR26" s="9"/>
+      <c r="AS26" s="9"/>
+      <c r="AT26" s="9"/>
+      <c r="AU26" s="9"/>
+      <c r="AV26" s="9"/>
+      <c r="AW26" s="9"/>
+      <c r="AX26" s="9"/>
+      <c r="AY26" s="9"/>
+      <c r="BA26" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB26" s="9"/>
+      <c r="BC26" s="9"/>
+      <c r="BD26" s="9"/>
+      <c r="BE26" s="9"/>
+      <c r="BF26" s="9"/>
+      <c r="BG26" s="9"/>
+      <c r="BH26" s="9"/>
+      <c r="BI26" s="9"/>
+      <c r="BK26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="BL26" s="9"/>
+      <c r="BM26" s="9"/>
+      <c r="BN26" s="9"/>
+      <c r="BO26" s="9"/>
+      <c r="BP26" s="9"/>
+      <c r="BQ26" s="9"/>
+      <c r="BR26" s="9"/>
+      <c r="BS26" s="9"/>
     </row>
     <row r="27" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W27" s="7" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3">
+        <f>BC23/BA18</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <f>BD23</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <f>BE23</f>
+        <v>-46.4</v>
+      </c>
+      <c r="G27" s="1">
+        <f>BF23</f>
+        <v>-48</v>
+      </c>
+      <c r="H27" s="1">
+        <f>BH23</f>
+        <v>159.4</v>
+      </c>
+      <c r="I27" s="1">
+        <f>BI23</f>
+        <v>32.494</v>
+      </c>
+      <c r="W27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
-      <c r="AA27" s="7"/>
-      <c r="AB27" s="7"/>
-      <c r="AC27" s="8" t="s">
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8"/>
+      <c r="AB27" s="8"/>
+      <c r="AC27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AG27" s="7" t="s">
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AG27" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AH27" s="7"/>
-      <c r="AI27" s="7"/>
-      <c r="AJ27" s="7"/>
-      <c r="AK27" s="7"/>
-      <c r="AL27" s="7"/>
-      <c r="AM27" s="8" t="s">
+      <c r="AH27" s="8"/>
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="8"/>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="8"/>
+      <c r="AM27" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AN27" s="8"/>
-      <c r="AO27" s="8"/>
+      <c r="AN27" s="9"/>
+      <c r="AO27" s="9"/>
+      <c r="AQ27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR27" s="8"/>
+      <c r="AS27" s="8"/>
+      <c r="AT27" s="8"/>
+      <c r="AU27" s="8"/>
+      <c r="AV27" s="8"/>
+      <c r="AW27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX27" s="9"/>
+      <c r="AY27" s="9"/>
+      <c r="BA27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB27" s="8"/>
+      <c r="BC27" s="8"/>
+      <c r="BD27" s="8"/>
+      <c r="BE27" s="8"/>
+      <c r="BF27" s="8"/>
+      <c r="BG27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BH27" s="9"/>
+      <c r="BI27" s="9"/>
+      <c r="BK27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="BL27" s="8"/>
+      <c r="BM27" s="8"/>
+      <c r="BN27" s="8"/>
+      <c r="BO27" s="8"/>
+      <c r="BP27" s="8"/>
+      <c r="BQ27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="BR27" s="9"/>
+      <c r="BS27" s="9"/>
     </row>
     <row r="28" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W28" s="7" t="s">
+      <c r="W28" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="X28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="7" t="s">
+      <c r="X28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="Z28" s="7" t="s">
+      <c r="Z28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AA28" s="8" t="s">
+      <c r="AA28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AB28" s="8"/>
-      <c r="AC28" s="7" t="s">
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AD28" s="7" t="s">
+      <c r="AD28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AE28" s="7" t="s">
+      <c r="AE28" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AG28" s="7" t="s">
+      <c r="AG28" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="AH28" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="7" t="s">
+      <c r="AH28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="AJ28" s="7" t="s">
+      <c r="AJ28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AK28" s="8" t="s">
+      <c r="AK28" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AL28" s="8"/>
-      <c r="AM28" s="7" t="s">
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AN28" s="7" t="s">
+      <c r="AN28" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AO28" s="7" t="s">
+      <c r="AO28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV28" s="9"/>
+      <c r="AW28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AY28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BB28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF28" s="9"/>
+      <c r="BG28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BH28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI28" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="BK28" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BL28" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="BM28" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="BN28" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP28" s="9"/>
+      <c r="BQ28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="BS28" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W29" s="7"/>
-      <c r="X29" s="7"/>
-      <c r="Y29" s="7"/>
-      <c r="Z29" s="7"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8"/>
+      <c r="Y29" s="8"/>
+      <c r="Z29" s="8"/>
       <c r="AA29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AB29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
-      <c r="AG29" s="7"/>
-      <c r="AH29" s="7"/>
-      <c r="AI29" s="7"/>
-      <c r="AJ29" s="7"/>
+      <c r="AC29" s="8"/>
+      <c r="AD29" s="8"/>
+      <c r="AE29" s="8"/>
+      <c r="AG29" s="8"/>
+      <c r="AH29" s="8"/>
+      <c r="AI29" s="8"/>
+      <c r="AJ29" s="8"/>
       <c r="AK29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="AL29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AM29" s="7"/>
-      <c r="AN29" s="7"/>
-      <c r="AO29" s="7"/>
+      <c r="AM29" s="8"/>
+      <c r="AN29" s="8"/>
+      <c r="AO29" s="8"/>
+      <c r="AQ29" s="8"/>
+      <c r="AR29" s="8"/>
+      <c r="AS29" s="8"/>
+      <c r="AT29" s="8"/>
+      <c r="AU29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW29" s="8"/>
+      <c r="AX29" s="8"/>
+      <c r="AY29" s="8"/>
+      <c r="BA29" s="8"/>
+      <c r="BB29" s="8"/>
+      <c r="BC29" s="8"/>
+      <c r="BD29" s="8"/>
+      <c r="BE29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG29" s="8"/>
+      <c r="BH29" s="8"/>
+      <c r="BI29" s="8"/>
+      <c r="BK29" s="8"/>
+      <c r="BL29" s="8"/>
+      <c r="BM29" s="8"/>
+      <c r="BN29" s="8"/>
+      <c r="BO29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="BP29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ29" s="8"/>
+      <c r="BR29" s="8"/>
+      <c r="BS29" s="8"/>
     </row>
     <row r="30" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W30" s="6">
+      <c r="W30" s="7">
         <v>40</v>
       </c>
       <c r="X30" s="1">
@@ -7070,7 +8399,7 @@
       <c r="AB30" s="1">
         <v>-41</v>
       </c>
-      <c r="AC30" s="6">
+      <c r="AC30" s="7">
         <v>10</v>
       </c>
       <c r="AD30" s="1">
@@ -7079,7 +8408,7 @@
       <c r="AE30" s="1">
         <v>10.23</v>
       </c>
-      <c r="AG30" s="6">
+      <c r="AG30" s="7">
         <v>40</v>
       </c>
       <c r="AH30" s="1">
@@ -7097,7 +8426,7 @@
       <c r="AL30" s="1">
         <v>-55</v>
       </c>
-      <c r="AM30" s="6">
+      <c r="AM30" s="7">
         <v>10</v>
       </c>
       <c r="AN30" s="1">
@@ -7106,9 +8435,62 @@
       <c r="AO30" s="1">
         <v>10.29</v>
       </c>
+      <c r="AQ30" s="7">
+        <v>40</v>
+      </c>
+      <c r="AR30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS30" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT30" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU30" s="1">
+        <v>-57</v>
+      </c>
+      <c r="AV30" s="1">
+        <v>-53</v>
+      </c>
+      <c r="AW30" s="7">
+        <v>10</v>
+      </c>
+      <c r="AX30" s="1">
+        <v>147</v>
+      </c>
+      <c r="AY30" s="1">
+        <v>29.15</v>
+      </c>
+      <c r="BA30" s="7">
+        <v>40</v>
+      </c>
+      <c r="BB30" s="1"/>
+      <c r="BC30" s="1"/>
+      <c r="BD30" s="1"/>
+      <c r="BE30" s="1"/>
+      <c r="BF30" s="1"/>
+      <c r="BG30" s="7">
+        <v>10</v>
+      </c>
+      <c r="BH30" s="1"/>
+      <c r="BI30" s="1"/>
+      <c r="BK30" s="7">
+        <v>40</v>
+      </c>
+      <c r="BL30" s="1"/>
+      <c r="BM30" s="1"/>
+      <c r="BN30" s="1"/>
+      <c r="BO30" s="1"/>
+      <c r="BP30" s="1"/>
+      <c r="BQ30" s="7">
+        <v>10</v>
+      </c>
+      <c r="BR30" s="1"/>
+      <c r="BS30" s="1"/>
     </row>
     <row r="31" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W31" s="6"/>
+      <c r="W31" s="7"/>
       <c r="X31" s="1">
         <v>0</v>
       </c>
@@ -7124,14 +8506,14 @@
       <c r="AB31" s="1">
         <v>-41</v>
       </c>
-      <c r="AC31" s="6"/>
+      <c r="AC31" s="7"/>
       <c r="AD31" s="1">
         <v>51</v>
       </c>
       <c r="AE31" s="1">
         <v>10.25</v>
       </c>
-      <c r="AG31" s="6"/>
+      <c r="AG31" s="7"/>
       <c r="AH31" s="1">
         <v>0</v>
       </c>
@@ -7147,16 +8529,57 @@
       <c r="AL31" s="1">
         <v>-58</v>
       </c>
-      <c r="AM31" s="6"/>
+      <c r="AM31" s="7"/>
       <c r="AN31" s="1">
         <v>43</v>
       </c>
       <c r="AO31" s="1">
         <v>8.6999999999999993</v>
       </c>
+      <c r="AQ31" s="7"/>
+      <c r="AR31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS31" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT31" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU31" s="1">
+        <v>-55</v>
+      </c>
+      <c r="AV31" s="1">
+        <v>-56</v>
+      </c>
+      <c r="AW31" s="7"/>
+      <c r="AX31" s="1">
+        <v>141</v>
+      </c>
+      <c r="AY31" s="1">
+        <v>28.75</v>
+      </c>
+      <c r="BA31" s="7"/>
+      <c r="BB31" s="1"/>
+      <c r="BC31" s="1"/>
+      <c r="BD31" s="1"/>
+      <c r="BE31" s="1"/>
+      <c r="BF31" s="1"/>
+      <c r="BG31" s="7"/>
+      <c r="BH31" s="1"/>
+      <c r="BI31" s="1"/>
+      <c r="BK31" s="7"/>
+      <c r="BL31" s="1"/>
+      <c r="BM31" s="1"/>
+      <c r="BN31" s="1"/>
+      <c r="BO31" s="1"/>
+      <c r="BP31" s="1"/>
+      <c r="BQ31" s="7"/>
+      <c r="BR31" s="1"/>
+      <c r="BS31" s="1"/>
     </row>
     <row r="32" spans="2:92" x14ac:dyDescent="0.2">
-      <c r="W32" s="6"/>
+      <c r="W32" s="7"/>
       <c r="X32" s="1">
         <v>0</v>
       </c>
@@ -7172,14 +8595,14 @@
       <c r="AB32" s="1">
         <v>-42</v>
       </c>
-      <c r="AC32" s="6"/>
+      <c r="AC32" s="7"/>
       <c r="AD32" s="1">
         <v>51</v>
       </c>
       <c r="AE32" s="1">
         <v>10.41</v>
       </c>
-      <c r="AG32" s="6"/>
+      <c r="AG32" s="7"/>
       <c r="AH32" s="1">
         <v>0</v>
       </c>
@@ -7195,16 +8618,57 @@
       <c r="AL32" s="1">
         <v>-59</v>
       </c>
-      <c r="AM32" s="6"/>
+      <c r="AM32" s="7"/>
       <c r="AN32" s="1">
         <v>51</v>
       </c>
       <c r="AO32" s="1">
         <v>10.3</v>
       </c>
+      <c r="AQ32" s="7"/>
+      <c r="AR32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS32" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU32" s="1">
+        <v>-51</v>
+      </c>
+      <c r="AV32" s="1">
+        <v>-54</v>
+      </c>
+      <c r="AW32" s="7"/>
+      <c r="AX32" s="1">
+        <v>141</v>
+      </c>
+      <c r="AY32" s="1">
+        <v>28.52</v>
+      </c>
+      <c r="BA32" s="7"/>
+      <c r="BB32" s="1"/>
+      <c r="BC32" s="1"/>
+      <c r="BD32" s="1"/>
+      <c r="BE32" s="1"/>
+      <c r="BF32" s="1"/>
+      <c r="BG32" s="7"/>
+      <c r="BH32" s="1"/>
+      <c r="BI32" s="1"/>
+      <c r="BK32" s="7"/>
+      <c r="BL32" s="1"/>
+      <c r="BM32" s="1"/>
+      <c r="BN32" s="1"/>
+      <c r="BO32" s="1"/>
+      <c r="BP32" s="1"/>
+      <c r="BQ32" s="7"/>
+      <c r="BR32" s="1"/>
+      <c r="BS32" s="1"/>
     </row>
-    <row r="33" spans="23:41" x14ac:dyDescent="0.2">
-      <c r="W33" s="6"/>
+    <row r="33" spans="23:71" x14ac:dyDescent="0.2">
+      <c r="W33" s="7"/>
       <c r="X33" s="1">
         <v>0</v>
       </c>
@@ -7220,14 +8684,14 @@
       <c r="AB33" s="1">
         <v>-42</v>
       </c>
-      <c r="AC33" s="6"/>
+      <c r="AC33" s="7"/>
       <c r="AD33" s="1">
         <v>51</v>
       </c>
       <c r="AE33" s="1">
         <v>8.3699999999999992</v>
       </c>
-      <c r="AG33" s="6"/>
+      <c r="AG33" s="7"/>
       <c r="AH33" s="1">
         <v>0</v>
       </c>
@@ -7243,16 +8707,57 @@
       <c r="AL33" s="1">
         <v>-53</v>
       </c>
-      <c r="AM33" s="6"/>
+      <c r="AM33" s="7"/>
       <c r="AN33" s="1">
         <v>48</v>
       </c>
       <c r="AO33" s="1">
         <v>9.66</v>
       </c>
+      <c r="AQ33" s="7"/>
+      <c r="AR33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS33" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT33" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU33" s="1">
+        <v>-54</v>
+      </c>
+      <c r="AV33" s="1">
+        <v>-59</v>
+      </c>
+      <c r="AW33" s="7"/>
+      <c r="AX33" s="1">
+        <v>157</v>
+      </c>
+      <c r="AY33" s="1">
+        <v>31.93</v>
+      </c>
+      <c r="BA33" s="7"/>
+      <c r="BB33" s="1"/>
+      <c r="BC33" s="1"/>
+      <c r="BD33" s="1"/>
+      <c r="BE33" s="1"/>
+      <c r="BF33" s="1"/>
+      <c r="BG33" s="7"/>
+      <c r="BH33" s="1"/>
+      <c r="BI33" s="1"/>
+      <c r="BK33" s="7"/>
+      <c r="BL33" s="1"/>
+      <c r="BM33" s="1"/>
+      <c r="BN33" s="1"/>
+      <c r="BO33" s="1"/>
+      <c r="BP33" s="1"/>
+      <c r="BQ33" s="7"/>
+      <c r="BR33" s="1"/>
+      <c r="BS33" s="1"/>
     </row>
-    <row r="34" spans="23:41" x14ac:dyDescent="0.2">
-      <c r="W34" s="6"/>
+    <row r="34" spans="23:71" x14ac:dyDescent="0.2">
+      <c r="W34" s="7"/>
       <c r="X34" s="1">
         <v>0</v>
       </c>
@@ -7268,14 +8773,14 @@
       <c r="AB34" s="1">
         <v>-44</v>
       </c>
-      <c r="AC34" s="6"/>
+      <c r="AC34" s="7"/>
       <c r="AD34" s="1">
         <v>51</v>
       </c>
       <c r="AE34" s="1">
         <v>10.38</v>
       </c>
-      <c r="AG34" s="6"/>
+      <c r="AG34" s="7"/>
       <c r="AH34" s="1">
         <v>0</v>
       </c>
@@ -7291,15 +8796,56 @@
       <c r="AL34" s="1">
         <v>-52</v>
       </c>
-      <c r="AM34" s="6"/>
+      <c r="AM34" s="7"/>
       <c r="AN34" s="1">
         <v>50</v>
       </c>
       <c r="AO34" s="1">
         <v>9.86</v>
       </c>
+      <c r="AQ34" s="7"/>
+      <c r="AR34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS34" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU34" s="1">
+        <v>-50</v>
+      </c>
+      <c r="AV34" s="1">
+        <v>-61</v>
+      </c>
+      <c r="AW34" s="7"/>
+      <c r="AX34" s="1">
+        <v>151</v>
+      </c>
+      <c r="AY34" s="1">
+        <v>30.91</v>
+      </c>
+      <c r="BA34" s="7"/>
+      <c r="BB34" s="1"/>
+      <c r="BC34" s="1"/>
+      <c r="BD34" s="1"/>
+      <c r="BE34" s="1"/>
+      <c r="BF34" s="1"/>
+      <c r="BG34" s="7"/>
+      <c r="BH34" s="1"/>
+      <c r="BI34" s="1"/>
+      <c r="BK34" s="7"/>
+      <c r="BL34" s="1"/>
+      <c r="BM34" s="1"/>
+      <c r="BN34" s="1"/>
+      <c r="BO34" s="1"/>
+      <c r="BP34" s="1"/>
+      <c r="BQ34" s="7"/>
+      <c r="BR34" s="1"/>
+      <c r="BS34" s="1"/>
     </row>
-    <row r="35" spans="23:41" x14ac:dyDescent="0.2">
+    <row r="35" spans="23:71" x14ac:dyDescent="0.2">
       <c r="W35" s="2" t="s">
         <v>15</v>
       </c>
@@ -7308,30 +8854,30 @@
         <v>0</v>
       </c>
       <c r="Y35" s="2">
-        <f t="shared" ref="Y35" si="27">SUM(Y30:Y34)/(5-COUNTBLANK(Y30:Y34))</f>
+        <f t="shared" ref="Y35" si="37">SUM(Y30:Y34)/(5-COUNTBLANK(Y30:Y34))</f>
         <v>40</v>
       </c>
       <c r="Z35" s="2">
-        <f t="shared" ref="Z35" si="28">SUM(Z30:Z34)/(5-COUNTBLANK(Z30:Z34))</f>
+        <f t="shared" ref="Z35" si="38">SUM(Z30:Z34)/(5-COUNTBLANK(Z30:Z34))</f>
         <v>0</v>
       </c>
       <c r="AA35" s="2">
-        <f t="shared" ref="AA35" si="29">SUM(AA30:AA34)/(5-COUNTBLANK(AA30:AA34))</f>
+        <f t="shared" ref="AA35" si="39">SUM(AA30:AA34)/(5-COUNTBLANK(AA30:AA34))</f>
         <v>-40</v>
       </c>
       <c r="AB35" s="2">
-        <f t="shared" ref="AB35" si="30">SUM(AB30:AB34)/(5-COUNTBLANK(AB30:AB34))</f>
+        <f t="shared" ref="AB35" si="40">SUM(AB30:AB34)/(5-COUNTBLANK(AB30:AB34))</f>
         <v>-42</v>
       </c>
       <c r="AC35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="AD35" s="2">
-        <f t="shared" ref="AD35" si="31">SUM(AD30:AD34)/(5-COUNTBLANK(AD30:AD34))</f>
+        <f t="shared" ref="AD35" si="41">SUM(AD30:AD34)/(5-COUNTBLANK(AD30:AD34))</f>
         <v>51</v>
       </c>
       <c r="AE35" s="2">
-        <f t="shared" ref="AE35" si="32">SUM(AE30:AE34)/(5-COUNTBLANK(AE30:AE34))</f>
+        <f t="shared" ref="AE35" si="42">SUM(AE30:AE34)/(5-COUNTBLANK(AE30:AE34))</f>
         <v>9.9280000000000008</v>
       </c>
       <c r="AG35" s="2" t="s">
@@ -7342,35 +8888,138 @@
         <v>0</v>
       </c>
       <c r="AI35" s="2">
-        <f t="shared" ref="AI35" si="33">SUM(AI30:AI34)/(5-COUNTBLANK(AI30:AI34))</f>
+        <f t="shared" ref="AI35" si="43">SUM(AI30:AI34)/(5-COUNTBLANK(AI30:AI34))</f>
         <v>40</v>
       </c>
       <c r="AJ35" s="2">
-        <f t="shared" ref="AJ35" si="34">SUM(AJ30:AJ34)/(5-COUNTBLANK(AJ30:AJ34))</f>
+        <f t="shared" ref="AJ35" si="44">SUM(AJ30:AJ34)/(5-COUNTBLANK(AJ30:AJ34))</f>
         <v>0</v>
       </c>
       <c r="AK35" s="2">
-        <f t="shared" ref="AK35" si="35">SUM(AK30:AK34)/(5-COUNTBLANK(AK30:AK34))</f>
+        <f t="shared" ref="AK35" si="45">SUM(AK30:AK34)/(5-COUNTBLANK(AK30:AK34))</f>
         <v>-55.2</v>
       </c>
       <c r="AL35" s="2">
-        <f t="shared" ref="AL35" si="36">SUM(AL30:AL34)/(5-COUNTBLANK(AL30:AL34))</f>
+        <f t="shared" ref="AL35" si="46">SUM(AL30:AL34)/(5-COUNTBLANK(AL30:AL34))</f>
         <v>-55.4</v>
       </c>
       <c r="AM35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="AN35" s="2">
-        <f t="shared" ref="AN35" si="37">SUM(AN30:AN34)/(5-COUNTBLANK(AN30:AN34))</f>
+        <f t="shared" ref="AN35" si="47">SUM(AN30:AN34)/(5-COUNTBLANK(AN30:AN34))</f>
         <v>48.6</v>
       </c>
       <c r="AO35" s="2">
-        <f t="shared" ref="AO35" si="38">SUM(AO30:AO34)/(5-COUNTBLANK(AO30:AO34))</f>
+        <f t="shared" ref="AO35" si="48">SUM(AO30:AO34)/(5-COUNTBLANK(AO30:AO34))</f>
         <v>9.7620000000000005</v>
+      </c>
+      <c r="AQ35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR35" s="6">
+        <f>SUM(AR30:AR34)/(5-COUNTBLANK(AR30:AR34))</f>
+        <v>0</v>
+      </c>
+      <c r="AS35" s="6">
+        <f t="shared" ref="AS35:AV35" si="49">SUM(AS30:AS34)/(5-COUNTBLANK(AS30:AS34))</f>
+        <v>40</v>
+      </c>
+      <c r="AT35" s="6">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="AU35" s="6">
+        <f t="shared" si="49"/>
+        <v>-53.4</v>
+      </c>
+      <c r="AV35" s="6">
+        <f t="shared" si="49"/>
+        <v>-56.6</v>
+      </c>
+      <c r="AW35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX35" s="6">
+        <f t="shared" ref="AX35:AY35" si="50">SUM(AX30:AX34)/(5-COUNTBLANK(AX30:AX34))</f>
+        <v>147.4</v>
+      </c>
+      <c r="AY35" s="6">
+        <f t="shared" si="50"/>
+        <v>29.851999999999997</v>
+      </c>
+      <c r="BA35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB35" s="6" t="e">
+        <f>SUM(BB30:BB34)/(5-COUNTBLANK(BB30:BB34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BC35" s="6" t="e">
+        <f t="shared" ref="BC35:BF35" si="51">SUM(BC30:BC34)/(5-COUNTBLANK(BC30:BC34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BD35" s="6" t="e">
+        <f t="shared" si="51"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BE35" s="6" t="e">
+        <f t="shared" si="51"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BF35" s="6" t="e">
+        <f t="shared" si="51"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BG35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH35" s="6" t="e">
+        <f t="shared" ref="BH35:BI35" si="52">SUM(BH30:BH34)/(5-COUNTBLANK(BH30:BH34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BI35" s="6" t="e">
+        <f t="shared" si="52"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BK35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="BL35" s="6" t="e">
+        <f>SUM(BL30:BL34)/(5-COUNTBLANK(BL30:BL34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BM35" s="6" t="e">
+        <f t="shared" ref="BM35:BP35" si="53">SUM(BM30:BM34)/(5-COUNTBLANK(BM30:BM34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BN35" s="6" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BO35" s="6" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BP35" s="6" t="e">
+        <f t="shared" si="53"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BQ35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="BR35" s="6" t="e">
+        <f t="shared" ref="BR35:BS35" si="54">SUM(BR30:BR34)/(5-COUNTBLANK(BR30:BR34))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="BS35" s="6" t="e">
+        <f t="shared" si="54"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="146">
+  <mergeCells count="250">
+    <mergeCell ref="B17:B27"/>
     <mergeCell ref="AG30:AG34"/>
     <mergeCell ref="AM30:AM34"/>
     <mergeCell ref="AG14:AO14"/>
@@ -7417,8 +9066,6 @@
     <mergeCell ref="Z28:Z29"/>
     <mergeCell ref="AG18:AG22"/>
     <mergeCell ref="AM18:AM22"/>
-    <mergeCell ref="W18:W22"/>
-    <mergeCell ref="AC18:AC22"/>
     <mergeCell ref="W2:AE2"/>
     <mergeCell ref="W3:AB3"/>
     <mergeCell ref="AC3:AE3"/>
@@ -7430,7 +9077,6 @@
     <mergeCell ref="AC4:AC5"/>
     <mergeCell ref="AD4:AD5"/>
     <mergeCell ref="AE4:AE5"/>
-    <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="AA28:AB28"/>
@@ -7454,16 +9100,29 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="M6:M10"/>
-    <mergeCell ref="S6:S10"/>
+    <mergeCell ref="W18:W22"/>
     <mergeCell ref="Y4:Y5"/>
     <mergeCell ref="Z4:Z5"/>
     <mergeCell ref="AQ6:AQ10"/>
     <mergeCell ref="AW6:AW10"/>
     <mergeCell ref="CF20:CF24"/>
     <mergeCell ref="CL20:CL24"/>
-    <mergeCell ref="B17:B23"/>
+    <mergeCell ref="AQ14:AY14"/>
+    <mergeCell ref="AQ15:AV15"/>
+    <mergeCell ref="AW15:AY15"/>
+    <mergeCell ref="AQ16:AQ17"/>
+    <mergeCell ref="AR16:AR17"/>
+    <mergeCell ref="AS16:AS17"/>
+    <mergeCell ref="AT16:AT17"/>
+    <mergeCell ref="AU16:AV16"/>
+    <mergeCell ref="AW16:AW17"/>
+    <mergeCell ref="AX16:AX17"/>
+    <mergeCell ref="AY16:AY17"/>
+    <mergeCell ref="AQ18:AQ22"/>
+    <mergeCell ref="AW18:AW22"/>
+    <mergeCell ref="BH16:BH17"/>
+    <mergeCell ref="BI16:BI17"/>
+    <mergeCell ref="AC18:AC22"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="B15:B16"/>
@@ -7483,6 +9142,10 @@
     <mergeCell ref="I6:I10"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="M6:M10"/>
+    <mergeCell ref="S6:S10"/>
+    <mergeCell ref="J4:J5"/>
     <mergeCell ref="AQ2:AY2"/>
     <mergeCell ref="AQ3:AV3"/>
     <mergeCell ref="AW3:AY3"/>
@@ -7517,6 +9180,95 @@
     <mergeCell ref="CL18:CL19"/>
     <mergeCell ref="CM18:CM19"/>
     <mergeCell ref="CN18:CN19"/>
+    <mergeCell ref="AQ26:AY26"/>
+    <mergeCell ref="AQ27:AV27"/>
+    <mergeCell ref="AW27:AY27"/>
+    <mergeCell ref="AQ28:AQ29"/>
+    <mergeCell ref="AR28:AR29"/>
+    <mergeCell ref="AS28:AS29"/>
+    <mergeCell ref="AT28:AT29"/>
+    <mergeCell ref="AU28:AV28"/>
+    <mergeCell ref="AW28:AW29"/>
+    <mergeCell ref="AX28:AX29"/>
+    <mergeCell ref="AY28:AY29"/>
+    <mergeCell ref="AQ30:AQ34"/>
+    <mergeCell ref="AW30:AW34"/>
+    <mergeCell ref="BA2:BI2"/>
+    <mergeCell ref="BA3:BF3"/>
+    <mergeCell ref="BG3:BI3"/>
+    <mergeCell ref="BA4:BA5"/>
+    <mergeCell ref="BB4:BB5"/>
+    <mergeCell ref="BC4:BC5"/>
+    <mergeCell ref="BD4:BD5"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BG4:BG5"/>
+    <mergeCell ref="BH4:BH5"/>
+    <mergeCell ref="BI4:BI5"/>
+    <mergeCell ref="BA6:BA10"/>
+    <mergeCell ref="BG6:BG10"/>
+    <mergeCell ref="BA14:BI14"/>
+    <mergeCell ref="BA15:BF15"/>
+    <mergeCell ref="BG15:BI15"/>
+    <mergeCell ref="BA16:BA17"/>
+    <mergeCell ref="BB16:BB17"/>
+    <mergeCell ref="BC16:BC17"/>
+    <mergeCell ref="BD16:BD17"/>
+    <mergeCell ref="BE16:BF16"/>
+    <mergeCell ref="BG16:BG17"/>
+    <mergeCell ref="BA18:BA22"/>
+    <mergeCell ref="BG18:BG22"/>
+    <mergeCell ref="BA26:BI26"/>
+    <mergeCell ref="BA27:BF27"/>
+    <mergeCell ref="BG27:BI27"/>
+    <mergeCell ref="BA28:BA29"/>
+    <mergeCell ref="BB28:BB29"/>
+    <mergeCell ref="BC28:BC29"/>
+    <mergeCell ref="BD28:BD29"/>
+    <mergeCell ref="BE28:BF28"/>
+    <mergeCell ref="BG28:BG29"/>
+    <mergeCell ref="BH28:BH29"/>
+    <mergeCell ref="BI28:BI29"/>
+    <mergeCell ref="BA30:BA34"/>
+    <mergeCell ref="BG30:BG34"/>
+    <mergeCell ref="BK2:BS2"/>
+    <mergeCell ref="BK3:BP3"/>
+    <mergeCell ref="BQ3:BS3"/>
+    <mergeCell ref="BK4:BK5"/>
+    <mergeCell ref="BL4:BL5"/>
+    <mergeCell ref="BM4:BM5"/>
+    <mergeCell ref="BN4:BN5"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="BQ4:BQ5"/>
+    <mergeCell ref="BR4:BR5"/>
+    <mergeCell ref="BS4:BS5"/>
+    <mergeCell ref="BK6:BK10"/>
+    <mergeCell ref="BQ6:BQ10"/>
+    <mergeCell ref="BK14:BS14"/>
+    <mergeCell ref="BK15:BP15"/>
+    <mergeCell ref="BQ15:BS15"/>
+    <mergeCell ref="BK16:BK17"/>
+    <mergeCell ref="BL16:BL17"/>
+    <mergeCell ref="BM16:BM17"/>
+    <mergeCell ref="BN16:BN17"/>
+    <mergeCell ref="BO16:BP16"/>
+    <mergeCell ref="BQ16:BQ17"/>
+    <mergeCell ref="BK30:BK34"/>
+    <mergeCell ref="BQ30:BQ34"/>
+    <mergeCell ref="BR16:BR17"/>
+    <mergeCell ref="BS16:BS17"/>
+    <mergeCell ref="BK18:BK22"/>
+    <mergeCell ref="BQ18:BQ22"/>
+    <mergeCell ref="BK26:BS26"/>
+    <mergeCell ref="BK27:BP27"/>
+    <mergeCell ref="BQ27:BS27"/>
+    <mergeCell ref="BK28:BK29"/>
+    <mergeCell ref="BL28:BL29"/>
+    <mergeCell ref="BM28:BM29"/>
+    <mergeCell ref="BN28:BN29"/>
+    <mergeCell ref="BO28:BP28"/>
+    <mergeCell ref="BQ28:BQ29"/>
+    <mergeCell ref="BR28:BR29"/>
+    <mergeCell ref="BS28:BS29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>